<commit_message>
LLM description for each goal Fix error information for invalid function from llm Improvements to GUI part Allow for waiting running a goal, run in 2 min Fix error counter on CodeModule and ConditioModule Improve build info on DbModule Handle Parameters with different structure in DbModule Improve WriteExcelFile in FileModule StopListening added in FileModule Add AppendSystem, AppendAssistant and AppendUser to LllmModule AppendVariable and listen to variable improved reset to previous items in loop in LoopModule Support one item in LoopModule Many changes to UiModule and related MemoryStack set value using json path VariableHelper improvments Test for File Blog: InTheory Instant compile and Selfcorrecting software
</commit_message>
<xml_diff>
--- a/Tests/File/Employees.xlsx
+++ b/Tests/File/Employees.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rae2d92bddb1b49dab2a1cb591df32935"/>
+    <x:sheet name="Sheet1" sheetId="1" state="visible" r:id="Rce5ece2e1e09472c940730210e562a7d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -92,7 +92,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="5">
     <x:xf/>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>

</xml_diff>

<commit_message>
Changes for v0.1.0.14 (#45)
* LLM description for each goal
Fix error information for invalid function from llm
Improvements to GUI part
Allow for waiting running a goal, run in 2 min
Fix error counter on CodeModule and ConditioModule
Improve build info on DbModule
Handle Parameters with different structure in DbModule
Improve WriteExcelFile in FileModule
StopListening added in FileModule
Add AppendSystem, AppendAssistant and AppendUser to LllmModule
AppendVariable and listen to variable improved
reset to previous items in loop in LoopModule
Support one item in LoopModule
Many changes to UiModule and related
MemoryStack set value using json path
VariableHelper improvments
Test for File
Blog: InTheory Instant compile and Selfcorrecting software

* Update version on project files
</commit_message>
<xml_diff>
--- a/Tests/File/Employees.xlsx
+++ b/Tests/File/Employees.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rae2d92bddb1b49dab2a1cb591df32935"/>
+    <x:sheet name="Sheet1" sheetId="1" state="visible" r:id="Rce5ece2e1e09472c940730210e562a7d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -92,7 +92,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="5">
     <x:xf/>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>

</xml_diff>